<commit_message>
Add new testing files, make sure all row are filled.
</commit_message>
<xml_diff>
--- a/test/BattINFO_converter_standard_Excel_version_1.1.11.xlsx
+++ b/test/BattINFO_converter_standard_Excel_version_1.1.11.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nukp/Library/CloudStorage/Dropbox/PythonStuff/Empa/Notebooks/Empa_64 Fix Battinfo converter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nukp/Documents/Repository/BattInfoConverter/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E05D9D7-D922-E84B-B19C-00D333C67DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFF6290-1231-9943-923C-ADACC209433A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1460" yWindow="1660" windowWidth="42260" windowHeight="18860" xr2:uid="{1A6D523C-FE67-4F3F-AA9B-E9FEE83DA8F2}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="436">
   <si>
     <t>Metadata</t>
   </si>
@@ -1265,6 +1265,93 @@
   </si>
   <si>
     <t>hasConstituent-type|Spacer-hasMeasuredProperty-Thickness</t>
+  </si>
+  <si>
+    <t>test_value_row_84</t>
+  </si>
+  <si>
+    <t>test_value_row_85</t>
+  </si>
+  <si>
+    <t>test_value_row_86</t>
+  </si>
+  <si>
+    <t>test_value_row_87</t>
+  </si>
+  <si>
+    <t>test_value_row_88</t>
+  </si>
+  <si>
+    <t>test_value_row_89</t>
+  </si>
+  <si>
+    <t>test_value_row_90</t>
+  </si>
+  <si>
+    <t>test_value_row_91</t>
+  </si>
+  <si>
+    <t>test_value_row_112</t>
+  </si>
+  <si>
+    <t>test_value_row_113</t>
+  </si>
+  <si>
+    <t>test_value_row_114</t>
+  </si>
+  <si>
+    <t>test_value_row_115</t>
+  </si>
+  <si>
+    <t>test_value_row_116</t>
+  </si>
+  <si>
+    <t>test_value_row_117</t>
+  </si>
+  <si>
+    <t>test_value_row_118</t>
+  </si>
+  <si>
+    <t>test_value_row_119</t>
+  </si>
+  <si>
+    <t>test_value_row_120</t>
+  </si>
+  <si>
+    <t>test_value_row_121</t>
+  </si>
+  <si>
+    <t>test_value_row_122</t>
+  </si>
+  <si>
+    <t>test_value_row_123</t>
+  </si>
+  <si>
+    <t>test_value_row_124</t>
+  </si>
+  <si>
+    <t>test_value_row_44</t>
+  </si>
+  <si>
+    <t>test_value_row_45</t>
+  </si>
+  <si>
+    <t>test_value_row_46</t>
+  </si>
+  <si>
+    <t>test_value_row_47</t>
+  </si>
+  <si>
+    <t>test_value_row_48</t>
+  </si>
+  <si>
+    <t>test_value_row_49</t>
+  </si>
+  <si>
+    <t>test_value_row_50</t>
+  </si>
+  <si>
+    <t>test_value_row_51</t>
   </si>
 </sst>
 </file>
@@ -1478,7 +1565,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1657,6 +1744,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2349,13 +2439,13 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:KA153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E143" sqref="E143"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="71.796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="75.19921875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="94.59765625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.19921875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.3984375" style="10" bestFit="1" customWidth="1"/>
@@ -3489,6 +3579,9 @@
       <c r="A44" s="2" t="s">
         <v>102</v>
       </c>
+      <c r="B44" s="4" t="s">
+        <v>428</v>
+      </c>
       <c r="C44" s="4" t="s">
         <v>9</v>
       </c>
@@ -3503,7 +3596,9 @@
       <c r="A45" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B45" s="6"/>
+      <c r="B45" s="6" t="s">
+        <v>429</v>
+      </c>
       <c r="C45" s="6" t="s">
         <v>9</v>
       </c>
@@ -3519,6 +3614,9 @@
       <c r="A46" s="2" t="s">
         <v>106</v>
       </c>
+      <c r="B46" s="4" t="s">
+        <v>430</v>
+      </c>
       <c r="C46" s="4" t="s">
         <v>9</v>
       </c>
@@ -3533,7 +3631,9 @@
       <c r="A47" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B47" s="6"/>
+      <c r="B47" s="6" t="s">
+        <v>431</v>
+      </c>
       <c r="C47" s="6" t="s">
         <v>9</v>
       </c>
@@ -3549,6 +3649,9 @@
       <c r="A48" s="2" t="s">
         <v>110</v>
       </c>
+      <c r="B48" s="4" t="s">
+        <v>432</v>
+      </c>
       <c r="C48" s="4" t="s">
         <v>9</v>
       </c>
@@ -3563,7 +3666,9 @@
       <c r="A49" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B49" s="6"/>
+      <c r="B49" s="6" t="s">
+        <v>433</v>
+      </c>
       <c r="C49" s="6" t="s">
         <v>9</v>
       </c>
@@ -3579,6 +3684,9 @@
       <c r="A50" s="2" t="s">
         <v>114</v>
       </c>
+      <c r="B50" s="4" t="s">
+        <v>434</v>
+      </c>
       <c r="C50" s="4" t="s">
         <v>9</v>
       </c>
@@ -3593,7 +3701,9 @@
       <c r="A51" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B51" s="6"/>
+      <c r="B51" s="6" t="s">
+        <v>435</v>
+      </c>
       <c r="C51" s="6" t="s">
         <v>9</v>
       </c>
@@ -4145,6 +4255,9 @@
       <c r="A84" s="2" t="s">
         <v>169</v>
       </c>
+      <c r="B84" s="4" t="s">
+        <v>407</v>
+      </c>
       <c r="C84" s="4" t="s">
         <v>9</v>
       </c>
@@ -4159,7 +4272,9 @@
       <c r="A85" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="B85" s="8"/>
+      <c r="B85" s="8" t="s">
+        <v>408</v>
+      </c>
       <c r="C85" s="8" t="s">
         <v>9</v>
       </c>
@@ -4175,6 +4290,9 @@
       <c r="A86" s="2" t="s">
         <v>173</v>
       </c>
+      <c r="B86" s="4" t="s">
+        <v>409</v>
+      </c>
       <c r="C86" s="4" t="s">
         <v>9</v>
       </c>
@@ -4189,7 +4307,9 @@
       <c r="A87" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="B87" s="8"/>
+      <c r="B87" s="8" t="s">
+        <v>410</v>
+      </c>
       <c r="C87" s="8" t="s">
         <v>9</v>
       </c>
@@ -4205,6 +4325,9 @@
       <c r="A88" s="2" t="s">
         <v>177</v>
       </c>
+      <c r="B88" s="4" t="s">
+        <v>411</v>
+      </c>
       <c r="C88" s="4" t="s">
         <v>9</v>
       </c>
@@ -4219,7 +4342,9 @@
       <c r="A89" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="B89" s="8"/>
+      <c r="B89" s="8" t="s">
+        <v>412</v>
+      </c>
       <c r="C89" s="8" t="s">
         <v>9</v>
       </c>
@@ -4235,6 +4360,9 @@
       <c r="A90" s="2" t="s">
         <v>181</v>
       </c>
+      <c r="B90" s="4" t="s">
+        <v>413</v>
+      </c>
       <c r="C90" s="4" t="s">
         <v>9</v>
       </c>
@@ -4249,7 +4377,9 @@
       <c r="A91" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="B91" s="8"/>
+      <c r="B91" s="8" t="s">
+        <v>414</v>
+      </c>
       <c r="C91" s="8" t="s">
         <v>9</v>
       </c>
@@ -4877,7 +5007,9 @@
       <c r="A112" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="B112" s="9"/>
+      <c r="B112" s="9" t="s">
+        <v>415</v>
+      </c>
       <c r="C112" s="9" t="s">
         <v>9</v>
       </c>
@@ -4893,6 +5025,9 @@
       <c r="A113" s="2" t="s">
         <v>230</v>
       </c>
+      <c r="B113" s="82" t="s">
+        <v>416</v>
+      </c>
       <c r="C113" s="4" t="s">
         <v>9</v>
       </c>
@@ -4907,7 +5042,9 @@
       <c r="A114" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="B114" s="9"/>
+      <c r="B114" s="9" t="s">
+        <v>417</v>
+      </c>
       <c r="C114" s="9" t="s">
         <v>9</v>
       </c>
@@ -4923,6 +5060,9 @@
       <c r="A115" s="2" t="s">
         <v>232</v>
       </c>
+      <c r="B115" s="82" t="s">
+        <v>418</v>
+      </c>
       <c r="C115" s="4" t="s">
         <v>9</v>
       </c>
@@ -4937,7 +5077,9 @@
       <c r="A116" s="76" t="s">
         <v>233</v>
       </c>
-      <c r="B116" s="77"/>
+      <c r="B116" s="9" t="s">
+        <v>419</v>
+      </c>
       <c r="C116" s="77" t="s">
         <v>9</v>
       </c>
@@ -4953,7 +5095,9 @@
       <c r="A117" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B117" s="74"/>
+      <c r="B117" s="82" t="s">
+        <v>420</v>
+      </c>
       <c r="C117" s="4" t="s">
         <v>9</v>
       </c>
@@ -4968,7 +5112,9 @@
       <c r="A118" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="B118" s="9"/>
+      <c r="B118" s="9" t="s">
+        <v>421</v>
+      </c>
       <c r="C118" s="9" t="s">
         <v>9</v>
       </c>
@@ -4984,6 +5130,9 @@
       <c r="A119" s="2" t="s">
         <v>236</v>
       </c>
+      <c r="B119" s="82" t="s">
+        <v>422</v>
+      </c>
       <c r="C119" s="4" t="s">
         <v>9</v>
       </c>
@@ -4998,7 +5147,9 @@
       <c r="A120" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="B120" s="9"/>
+      <c r="B120" s="9" t="s">
+        <v>423</v>
+      </c>
       <c r="C120" s="9" t="s">
         <v>9</v>
       </c>
@@ -5014,7 +5165,9 @@
       <c r="A121" s="62" t="s">
         <v>390</v>
       </c>
-      <c r="B121" s="79"/>
+      <c r="B121" s="82" t="s">
+        <v>424</v>
+      </c>
       <c r="C121" s="79" t="s">
         <v>9</v>
       </c>
@@ -5030,7 +5183,9 @@
       <c r="A122" s="11" t="s">
         <v>391</v>
       </c>
-      <c r="B122" s="9"/>
+      <c r="B122" s="9" t="s">
+        <v>425</v>
+      </c>
       <c r="C122" s="9" t="s">
         <v>9</v>
       </c>
@@ -5046,7 +5201,9 @@
       <c r="A123" s="62" t="s">
         <v>392</v>
       </c>
-      <c r="B123" s="79"/>
+      <c r="B123" s="82" t="s">
+        <v>426</v>
+      </c>
       <c r="C123" s="79" t="s">
         <v>9</v>
       </c>
@@ -5062,7 +5219,9 @@
       <c r="A124" s="11" t="s">
         <v>393</v>
       </c>
-      <c r="B124" s="9"/>
+      <c r="B124" s="9" t="s">
+        <v>427</v>
+      </c>
       <c r="C124" s="9" t="s">
         <v>9</v>
       </c>
@@ -9544,59 +9703,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <FolderType xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <CultureName xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Leaders xmlns="35345429-01ed-4d83-85b9-6cc21878d784">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Leaders>
-    <IsNotebookLocked xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Invited_Members xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Math_Settings xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Has_Leaders_Only_SectionGroup xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Member_Groups xmlns="35345429-01ed-4d83-85b9-6cc21878d784">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Member_Groups>
-    <Distribution_Groups xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <AppVersion xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Templates xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <NotebookType xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <TeamsChannelId xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Invited_Leaders xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Teams_Channel_Section_Location xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <Members xmlns="35345429-01ed-4d83-85b9-6cc21878d784">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Members>
-    <Owner xmlns="35345429-01ed-4d83-85b9-6cc21878d784">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <LMS_Mappings xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-    <_activity xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100F5BD758A7F2BF742ADB9291A93682A9E" ma:contentTypeVersion="31" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="0517f02299b6dbd064809d9c3f869e8a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="35345429-01ed-4d83-85b9-6cc21878d784" xmlns:ns4="53f86fb7-11c0-476e-bf8b-57768422e991" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a7ff6e993c77c55b2c02ebba747ae01b" ns3:_="" ns4:_="">
     <xsd:import namespace="35345429-01ed-4d83-85b9-6cc21878d784"/>
@@ -9993,6 +10099,59 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <FolderType xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <CultureName xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Leaders xmlns="35345429-01ed-4d83-85b9-6cc21878d784">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Leaders>
+    <IsNotebookLocked xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Invited_Members xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Math_Settings xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Has_Leaders_Only_SectionGroup xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Member_Groups xmlns="35345429-01ed-4d83-85b9-6cc21878d784">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Member_Groups>
+    <Distribution_Groups xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <AppVersion xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Templates xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <NotebookType xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <TeamsChannelId xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Invited_Leaders xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Teams_Channel_Section_Location xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <Members xmlns="35345429-01ed-4d83-85b9-6cc21878d784">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Members>
+    <Owner xmlns="35345429-01ed-4d83-85b9-6cc21878d784">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <LMS_Mappings xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+    <_activity xmlns="35345429-01ed-4d83-85b9-6cc21878d784" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E85C156E-EE0C-426A-92B3-CAF84DB17690}">
   <ds:schemaRefs>
@@ -10002,16 +10161,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2D89A20-922B-4399-8A99-02ABCC3D1E33}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="35345429-01ed-4d83-85b9-6cc21878d784"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D716C96-A80E-4732-A5D3-9C77E88EE8CA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10028,4 +10177,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2D89A20-922B-4399-8A99-02ABCC3D1E33}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="35345429-01ed-4d83-85b9-6cc21878d784"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>